<commit_message>
Fixed error in import file;
</commit_message>
<xml_diff>
--- a/hub/imports/fixtures/centers.xlsx
+++ b/hub/imports/fixtures/centers.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="960">
   <si>
     <t>Center Name</t>
   </si>
@@ -1692,9 +1692,6 @@
   </si>
   <si>
     <t>University of California, Los Angeles</t>
-  </si>
-  <si>
-    <t>Climate</t>
   </si>
   <si>
     <t>climate change, environmental focus</t>
@@ -3022,7 +3019,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="25" width="17.14"/>
+    <col customWidth="1" min="1" max="1" width="93.57"/>
+    <col customWidth="1" min="2" max="13" width="17.14"/>
+    <col customWidth="1" min="14" max="14" width="22.71"/>
+    <col customWidth="1" min="15" max="25" width="17.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8250,7 +8250,7 @@
         <v>24</v>
       </c>
       <c r="N109" s="4" t="s">
-        <v>554</v>
+        <v>252</v>
       </c>
       <c r="O109" s="6"/>
       <c r="P109" s="4" t="s">
@@ -8263,13 +8263,13 @@
         <v>123</v>
       </c>
       <c r="S109" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="T109" s="5">
         <v>2008.0</v>
       </c>
       <c r="U109" s="8" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="V109" s="9"/>
       <c r="W109" s="9"/>
@@ -8278,13 +8278,13 @@
     </row>
     <row r="110">
       <c r="A110" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="C110" s="4" t="s">
         <v>558</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>559</v>
       </c>
       <c r="D110" s="5">
         <v>18903.0</v>
@@ -8314,11 +8314,11 @@
         <v>123</v>
       </c>
       <c r="S110" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="T110" s="4"/>
       <c r="U110" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="V110" s="9"/>
       <c r="W110" s="9"/>
@@ -8327,13 +8327,13 @@
     </row>
     <row r="111">
       <c r="A111" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B111" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="B111" s="4" t="s">
-        <v>563</v>
-      </c>
       <c r="C111" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D111" s="5">
         <v>18903.0</v>
@@ -8361,13 +8361,13 @@
       </c>
       <c r="R111" s="4"/>
       <c r="S111" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="T111" s="5">
         <v>2011.0</v>
       </c>
       <c r="U111" s="8" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="V111" s="9"/>
       <c r="W111" s="9"/>
@@ -8376,13 +8376,13 @@
     </row>
     <row r="112">
       <c r="A112" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="C112" s="4" t="s">
         <v>567</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>568</v>
       </c>
       <c r="D112" s="5">
         <v>18922.0</v>
@@ -8410,11 +8410,11 @@
       </c>
       <c r="R112" s="4"/>
       <c r="S112" s="4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="T112" s="4"/>
       <c r="U112" s="8" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="V112" s="9"/>
       <c r="W112" s="9"/>
@@ -8423,10 +8423,10 @@
     </row>
     <row r="113">
       <c r="A113" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="B113" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>572</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>164</v>
@@ -8459,11 +8459,11 @@
         <v>123</v>
       </c>
       <c r="S113" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="T113" s="4"/>
       <c r="U113" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="V113" s="9"/>
       <c r="W113" s="9"/>
@@ -8472,13 +8472,13 @@
     </row>
     <row r="114">
       <c r="A114" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="B114" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="C114" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>577</v>
       </c>
       <c r="D114" s="5">
         <v>19141.0</v>
@@ -8506,13 +8506,13 @@
       </c>
       <c r="R114" s="4"/>
       <c r="S114" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="T114" s="5">
         <v>1978.0</v>
       </c>
       <c r="U114" s="8" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="V114" s="9"/>
       <c r="W114" s="9"/>
@@ -8521,13 +8521,13 @@
     </row>
     <row r="115">
       <c r="A115" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="B115" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="B115" s="4" t="s">
-        <v>581</v>
-      </c>
       <c r="C115" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D115" s="5">
         <v>19141.0</v>
@@ -8555,11 +8555,11 @@
       </c>
       <c r="R115" s="4"/>
       <c r="S115" s="4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="T115" s="4"/>
       <c r="U115" s="8" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="V115" s="9"/>
       <c r="W115" s="9"/>
@@ -8568,10 +8568,10 @@
     </row>
     <row r="116">
       <c r="A116" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>584</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>585</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>482</v>
@@ -8600,11 +8600,11 @@
       </c>
       <c r="R116" s="4"/>
       <c r="S116" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="T116" s="4"/>
       <c r="U116" s="8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="V116" s="9"/>
       <c r="W116" s="9"/>
@@ -8613,13 +8613,13 @@
     </row>
     <row r="117">
       <c r="A117" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="B117" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="C117" s="4" t="s">
         <v>589</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>590</v>
       </c>
       <c r="D117" s="5">
         <v>15168.0</v>
@@ -8645,11 +8645,11 @@
       <c r="Q117" s="4"/>
       <c r="R117" s="7"/>
       <c r="S117" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="T117" s="4"/>
       <c r="U117" s="8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="V117" s="9"/>
       <c r="W117" s="9"/>
@@ -8658,13 +8658,13 @@
     </row>
     <row r="118">
       <c r="A118" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="B118" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="C118" s="4" t="s">
         <v>594</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>595</v>
       </c>
       <c r="D118" s="5">
         <v>15253.0</v>
@@ -8690,11 +8690,11 @@
       <c r="Q118" s="4"/>
       <c r="R118" s="7"/>
       <c r="S118" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="T118" s="7"/>
       <c r="U118" s="8" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="V118" s="9"/>
       <c r="W118" s="9"/>
@@ -8703,13 +8703,13 @@
     </row>
     <row r="119">
       <c r="A119" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="B119" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="B119" s="4" t="s">
-        <v>599</v>
-      </c>
       <c r="C119" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D119" s="5">
         <v>15253.0</v>
@@ -8729,7 +8729,7 @@
         <v>99</v>
       </c>
       <c r="O119" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="P119" s="4" t="s">
         <v>87</v>
@@ -8737,11 +8737,11 @@
       <c r="Q119" s="4"/>
       <c r="R119" s="7"/>
       <c r="S119" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="T119" s="4"/>
       <c r="U119" s="8" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="V119" s="9"/>
       <c r="W119" s="9"/>
@@ -8750,10 +8750,10 @@
     </row>
     <row r="120">
       <c r="A120" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>603</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>604</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>169</v>
@@ -8782,11 +8782,11 @@
       <c r="Q120" s="4"/>
       <c r="R120" s="7"/>
       <c r="S120" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T120" s="7"/>
       <c r="U120" s="8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="V120" s="9"/>
       <c r="W120" s="9"/>
@@ -8795,13 +8795,13 @@
     </row>
     <row r="121">
       <c r="A121" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="B121" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="C121" s="4" t="s">
         <v>608</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>609</v>
       </c>
       <c r="D121" s="5">
         <v>15605.0</v>
@@ -8831,7 +8831,7 @@
       </c>
       <c r="T121" s="4"/>
       <c r="U121" s="8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="V121" s="9"/>
       <c r="W121" s="9"/>
@@ -8840,13 +8840,13 @@
     </row>
     <row r="122">
       <c r="A122" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="C122" s="4" t="s">
         <v>612</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>613</v>
       </c>
       <c r="D122" s="5">
         <v>15617.0</v>
@@ -8874,13 +8874,13 @@
       </c>
       <c r="R122" s="4"/>
       <c r="S122" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T122" s="5">
         <v>2009.0</v>
       </c>
       <c r="U122" s="8" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="V122" s="9"/>
       <c r="W122" s="9"/>
@@ -8889,13 +8889,13 @@
     </row>
     <row r="123">
       <c r="A123" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="B123" s="4" t="s">
-        <v>617</v>
-      </c>
       <c r="C123" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D123" s="5">
         <v>15617.0</v>
@@ -8923,11 +8923,11 @@
       </c>
       <c r="R123" s="4"/>
       <c r="S123" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T123" s="7"/>
       <c r="U123" s="8" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="V123" s="9"/>
       <c r="W123" s="9"/>
@@ -8936,13 +8936,13 @@
     </row>
     <row r="124">
       <c r="A124" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="B124" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="C124" s="4" t="s">
         <v>620</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>621</v>
       </c>
       <c r="D124" s="5">
         <v>15822.0</v>
@@ -8968,11 +8968,11 @@
       <c r="Q124" s="4"/>
       <c r="R124" s="7"/>
       <c r="S124" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T124" s="4"/>
       <c r="U124" s="8" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="V124" s="9"/>
       <c r="W124" s="9"/>
@@ -8981,13 +8981,13 @@
     </row>
     <row r="125">
       <c r="A125" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="B125" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="C125" s="4" t="s">
         <v>624</v>
-      </c>
-      <c r="C125" s="4" t="s">
-        <v>625</v>
       </c>
       <c r="D125" s="5">
         <v>15929.0</v>
@@ -9013,11 +9013,11 @@
       <c r="Q125" s="4"/>
       <c r="R125" s="7"/>
       <c r="S125" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="T125" s="4"/>
       <c r="U125" s="8" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="V125" s="9"/>
       <c r="W125" s="9"/>
@@ -9026,13 +9026,13 @@
     </row>
     <row r="126">
       <c r="A126" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>628</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="C126" s="4" t="s">
         <v>629</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>630</v>
       </c>
       <c r="D126" s="5">
         <v>19603.0</v>
@@ -9062,7 +9062,7 @@
       </c>
       <c r="T126" s="4"/>
       <c r="U126" s="8" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="V126" s="9"/>
       <c r="W126" s="9"/>
@@ -9071,13 +9071,13 @@
     </row>
     <row r="127">
       <c r="A127" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="B127" s="4" t="s">
         <v>632</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="C127" s="4" t="s">
         <v>633</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>634</v>
       </c>
       <c r="D127" s="5">
         <v>16228.0</v>
@@ -9103,11 +9103,11 @@
       <c r="Q127" s="4"/>
       <c r="R127" s="7"/>
       <c r="S127" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T127" s="4"/>
       <c r="U127" s="8" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="V127" s="9"/>
       <c r="W127" s="9"/>
@@ -9116,13 +9116,13 @@
     </row>
     <row r="128">
       <c r="A128" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="B128" s="4" t="s">
         <v>636</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="C128" s="4" t="s">
         <v>637</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>638</v>
       </c>
       <c r="D128" s="5">
         <v>16230.0</v>
@@ -9148,11 +9148,11 @@
       <c r="Q128" s="4"/>
       <c r="R128" s="7"/>
       <c r="S128" s="4" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="T128" s="4"/>
       <c r="U128" s="8" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="V128" s="9"/>
       <c r="W128" s="9"/>
@@ -9161,13 +9161,13 @@
     </row>
     <row r="129">
       <c r="A129" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="B129" s="4" t="s">
         <v>641</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="C129" s="4" t="s">
         <v>642</v>
-      </c>
-      <c r="C129" s="4" t="s">
-        <v>643</v>
       </c>
       <c r="D129" s="5">
         <v>16365.0</v>
@@ -9197,11 +9197,11 @@
       </c>
       <c r="R129" s="4"/>
       <c r="S129" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="T129" s="4"/>
       <c r="U129" s="8" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="V129" s="9"/>
       <c r="W129" s="9"/>
@@ -9210,13 +9210,13 @@
     </row>
     <row r="130">
       <c r="A130" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="B130" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="C130" s="4" t="s">
         <v>647</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>648</v>
       </c>
       <c r="D130" s="5">
         <v>16427.0</v>
@@ -9242,11 +9242,11 @@
       <c r="Q130" s="4"/>
       <c r="R130" s="7"/>
       <c r="S130" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="T130" s="4"/>
       <c r="U130" s="8" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="V130" s="9"/>
       <c r="W130" s="9"/>
@@ -9255,13 +9255,13 @@
     </row>
     <row r="131">
       <c r="A131" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B131" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="C131" s="4" t="s">
         <v>652</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>653</v>
       </c>
       <c r="D131" s="5">
         <v>16515.0</v>
@@ -9287,13 +9287,13 @@
       <c r="Q131" s="4"/>
       <c r="R131" s="7"/>
       <c r="S131" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T131" s="5">
         <v>2004.0</v>
       </c>
       <c r="U131" s="8" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="V131" s="9"/>
       <c r="W131" s="9"/>
@@ -9302,13 +9302,13 @@
     </row>
     <row r="132">
       <c r="A132" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="B132" s="4" t="s">
         <v>655</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="C132" s="4" t="s">
         <v>656</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>657</v>
       </c>
       <c r="D132" s="5">
         <v>16690.0</v>
@@ -9334,11 +9334,11 @@
       <c r="Q132" s="4"/>
       <c r="R132" s="7"/>
       <c r="S132" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="T132" s="4"/>
       <c r="U132" s="8" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="V132" s="9"/>
       <c r="W132" s="9"/>
@@ -9347,13 +9347,13 @@
     </row>
     <row r="133">
       <c r="A133" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="B133" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="C133" s="4" t="s">
         <v>661</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>662</v>
       </c>
       <c r="D133" s="5">
         <v>16747.0</v>
@@ -9379,13 +9379,13 @@
       <c r="Q133" s="4"/>
       <c r="R133" s="7"/>
       <c r="S133" s="4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="T133" s="5">
         <v>2007.0</v>
       </c>
       <c r="U133" s="8" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="V133" s="9"/>
       <c r="W133" s="9"/>
@@ -9394,13 +9394,13 @@
     </row>
     <row r="134">
       <c r="A134" s="4" t="s">
+        <v>664</v>
+      </c>
+      <c r="B134" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="C134" s="4" t="s">
         <v>666</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>667</v>
       </c>
       <c r="D134" s="5">
         <v>16798.0</v>
@@ -9428,11 +9428,11 @@
       </c>
       <c r="R134" s="7"/>
       <c r="S134" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="T134" s="4"/>
       <c r="U134" s="8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="V134" s="9"/>
       <c r="W134" s="9"/>
@@ -9441,13 +9441,13 @@
     </row>
     <row r="135">
       <c r="A135" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="B135" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="B135" s="4" t="s">
-        <v>671</v>
-      </c>
       <c r="C135" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D135" s="5">
         <v>16798.0</v>
@@ -9473,13 +9473,13 @@
       <c r="Q135" s="4"/>
       <c r="R135" s="7"/>
       <c r="S135" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T135" s="5">
         <v>1990.0</v>
       </c>
       <c r="U135" s="8" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="V135" s="9"/>
       <c r="W135" s="9"/>
@@ -9488,13 +9488,13 @@
     </row>
     <row r="136">
       <c r="A136" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="B136" s="4" t="s">
         <v>673</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="C136" s="4" t="s">
         <v>674</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>675</v>
       </c>
       <c r="D136" s="5">
         <v>16901.0</v>
@@ -9520,11 +9520,11 @@
       <c r="Q136" s="4"/>
       <c r="R136" s="7"/>
       <c r="S136" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T136" s="4"/>
       <c r="U136" s="8" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="V136" s="9"/>
       <c r="W136" s="9"/>
@@ -9533,13 +9533,13 @@
     </row>
     <row r="137">
       <c r="A137" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="B137" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="C137" s="4" t="s">
         <v>678</v>
-      </c>
-      <c r="C137" s="4" t="s">
-        <v>679</v>
       </c>
       <c r="D137" s="5">
         <v>17056.0</v>
@@ -9565,11 +9565,11 @@
       <c r="Q137" s="4"/>
       <c r="R137" s="7"/>
       <c r="S137" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T137" s="4"/>
       <c r="U137" s="8" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="V137" s="9"/>
       <c r="W137" s="9"/>
@@ -9578,10 +9578,10 @@
     </row>
     <row r="138">
       <c r="A138" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="B138" s="4" t="s">
         <v>681</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>682</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>468</v>
@@ -9610,11 +9610,11 @@
       <c r="Q138" s="4"/>
       <c r="R138" s="7"/>
       <c r="S138" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="T138" s="4"/>
       <c r="U138" s="8" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="V138" s="9"/>
       <c r="W138" s="9"/>
@@ -9623,10 +9623,10 @@
     </row>
     <row r="139">
       <c r="A139" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="B139" s="4" t="s">
         <v>685</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>686</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>468</v>
@@ -9655,11 +9655,11 @@
       <c r="Q139" s="4"/>
       <c r="R139" s="7"/>
       <c r="S139" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T139" s="7"/>
       <c r="U139" s="8" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="V139" s="9"/>
       <c r="W139" s="9"/>
@@ -9668,10 +9668,10 @@
     </row>
     <row r="140">
       <c r="A140" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="B140" s="4" t="s">
         <v>688</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>689</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>468</v>
@@ -9700,11 +9700,11 @@
       <c r="Q140" s="4"/>
       <c r="R140" s="7"/>
       <c r="S140" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T140" s="7"/>
       <c r="U140" s="8" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="V140" s="9"/>
       <c r="W140" s="9"/>
@@ -9713,10 +9713,10 @@
     </row>
     <row r="141">
       <c r="A141" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="B141" s="4" t="s">
         <v>691</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>692</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>468</v>
@@ -9745,11 +9745,11 @@
       <c r="Q141" s="4"/>
       <c r="R141" s="7"/>
       <c r="S141" s="4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="T141" s="7"/>
       <c r="U141" s="8" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V141" s="9"/>
       <c r="W141" s="9"/>
@@ -9758,13 +9758,13 @@
     </row>
     <row r="142">
       <c r="A142" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="B142" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="C142" s="4" t="s">
         <v>696</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>697</v>
       </c>
       <c r="D142" s="5">
         <v>17275.0</v>
@@ -9790,11 +9790,11 @@
       <c r="Q142" s="4"/>
       <c r="R142" s="7"/>
       <c r="S142" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="T142" s="4"/>
       <c r="U142" s="8" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="V142" s="9"/>
       <c r="W142" s="9"/>
@@ -9803,13 +9803,13 @@
     </row>
     <row r="143">
       <c r="A143" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="B143" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="C143" s="4" t="s">
         <v>701</v>
-      </c>
-      <c r="C143" s="4" t="s">
-        <v>702</v>
       </c>
       <c r="D143" s="5">
         <v>17306.0</v>
@@ -9835,11 +9835,11 @@
       <c r="Q143" s="4"/>
       <c r="R143" s="7"/>
       <c r="S143" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T143" s="4"/>
       <c r="U143" s="8" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="V143" s="9"/>
       <c r="W143" s="9"/>
@@ -9848,10 +9848,10 @@
     </row>
     <row r="144">
       <c r="A144" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="B144" s="4" t="s">
         <v>704</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>705</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>93</v>
@@ -9886,7 +9886,7 @@
         <v>2006.0</v>
       </c>
       <c r="U144" s="8" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="V144" s="9"/>
       <c r="W144" s="9"/>
@@ -9895,13 +9895,13 @@
     </row>
     <row r="145">
       <c r="A145" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="C145" s="4" t="s">
         <v>708</v>
-      </c>
-      <c r="C145" s="4" t="s">
-        <v>709</v>
       </c>
       <c r="D145" s="5">
         <v>17400.0</v>
@@ -9927,11 +9927,11 @@
       <c r="Q145" s="4"/>
       <c r="R145" s="7"/>
       <c r="S145" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="T145" s="4"/>
       <c r="U145" s="8" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="V145" s="9"/>
       <c r="W145" s="9"/>
@@ -9940,13 +9940,13 @@
     </row>
     <row r="146">
       <c r="A146" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="B146" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="C146" s="4" t="s">
         <v>713</v>
-      </c>
-      <c r="C146" s="4" t="s">
-        <v>714</v>
       </c>
       <c r="D146" s="5">
         <v>65947.0</v>
@@ -9972,13 +9972,13 @@
       <c r="Q146" s="4"/>
       <c r="R146" s="7"/>
       <c r="S146" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="T146" s="5">
         <v>2012.0</v>
       </c>
       <c r="U146" s="8" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="V146" s="9"/>
       <c r="W146" s="9"/>
@@ -9987,10 +9987,10 @@
     </row>
     <row r="147">
       <c r="A147" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>717</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>718</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>42</v>
@@ -10021,11 +10021,11 @@
       </c>
       <c r="R147" s="4"/>
       <c r="S147" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T147" s="4"/>
       <c r="U147" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="V147" s="9"/>
       <c r="W147" s="9"/>
@@ -10034,13 +10034,13 @@
     </row>
     <row r="148">
       <c r="A148" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="B148" s="4" t="s">
         <v>720</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="C148" s="4" t="s">
         <v>721</v>
-      </c>
-      <c r="C148" s="4" t="s">
-        <v>722</v>
       </c>
       <c r="D148" s="5">
         <v>17678.0</v>
@@ -10066,13 +10066,13 @@
       <c r="Q148" s="4"/>
       <c r="R148" s="7"/>
       <c r="S148" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="T148" s="5">
         <v>2007.0</v>
       </c>
       <c r="U148" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="V148" s="9"/>
       <c r="W148" s="9"/>
@@ -10081,13 +10081,13 @@
     </row>
     <row r="149">
       <c r="A149" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="B149" s="4" t="s">
         <v>725</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="C149" s="4" t="s">
         <v>726</v>
-      </c>
-      <c r="C149" s="4" t="s">
-        <v>727</v>
       </c>
       <c r="D149" s="5">
         <v>17758.0</v>
@@ -10113,11 +10113,11 @@
       <c r="Q149" s="4"/>
       <c r="R149" s="4"/>
       <c r="S149" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="T149" s="7"/>
       <c r="U149" s="8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="V149" s="9"/>
       <c r="W149" s="9"/>
@@ -10126,13 +10126,13 @@
     </row>
     <row r="150">
       <c r="A150" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="B150" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="B150" s="4" t="s">
-        <v>731</v>
-      </c>
       <c r="C150" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D150" s="5">
         <v>17758.0</v>
@@ -10158,11 +10158,11 @@
       <c r="Q150" s="4"/>
       <c r="R150" s="7"/>
       <c r="S150" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="T150" s="7"/>
       <c r="U150" s="8" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="V150" s="9"/>
       <c r="W150" s="9"/>
@@ -10171,10 +10171,10 @@
     </row>
     <row r="151">
       <c r="A151" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="B151" s="4" t="s">
         <v>734</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>735</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>535</v>
@@ -10205,11 +10205,11 @@
       </c>
       <c r="R151" s="4"/>
       <c r="S151" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="T151" s="4"/>
       <c r="U151" s="8" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="V151" s="9"/>
       <c r="W151" s="9"/>
@@ -10218,10 +10218,10 @@
     </row>
     <row r="152">
       <c r="A152" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="B152" s="4" t="s">
         <v>738</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>739</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>98</v>
@@ -10250,11 +10250,11 @@
       <c r="Q152" s="4"/>
       <c r="R152" s="7"/>
       <c r="S152" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="T152" s="7"/>
       <c r="U152" s="8" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="V152" s="9"/>
       <c r="W152" s="9"/>
@@ -10263,10 +10263,10 @@
     </row>
     <row r="153">
       <c r="A153" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="B153" s="4" t="s">
         <v>742</v>
-      </c>
-      <c r="B153" s="4" t="s">
-        <v>743</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>98</v>
@@ -10290,18 +10290,18 @@
       </c>
       <c r="O153" s="6"/>
       <c r="P153" s="4" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Q153" s="4" t="s">
         <v>87</v>
       </c>
       <c r="R153" s="4"/>
       <c r="S153" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T153" s="4"/>
       <c r="U153" s="8" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="V153" s="9"/>
       <c r="W153" s="9"/>
@@ -10310,13 +10310,13 @@
     </row>
     <row r="154">
       <c r="A154" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="B154" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="C154" s="4" t="s">
         <v>747</v>
-      </c>
-      <c r="C154" s="4" t="s">
-        <v>748</v>
       </c>
       <c r="D154" s="5">
         <v>21249.0</v>
@@ -10342,11 +10342,11 @@
       <c r="Q154" s="4"/>
       <c r="R154" s="7"/>
       <c r="S154" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T154" s="4"/>
       <c r="U154" s="8" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="V154" s="9"/>
       <c r="W154" s="9"/>
@@ -10355,13 +10355,13 @@
     </row>
     <row r="155">
       <c r="A155" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="B155" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="B155" s="4" t="s">
-        <v>751</v>
-      </c>
       <c r="C155" s="4" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D155" s="5">
         <v>21249.0</v>
@@ -10387,11 +10387,11 @@
       <c r="Q155" s="4"/>
       <c r="R155" s="7"/>
       <c r="S155" s="4" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="T155" s="7"/>
       <c r="U155" s="8" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="V155" s="9"/>
       <c r="W155" s="9"/>
@@ -10400,13 +10400,13 @@
     </row>
     <row r="156">
       <c r="A156" s="4" t="s">
+        <v>753</v>
+      </c>
+      <c r="B156" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="C156" s="4" t="s">
         <v>755</v>
-      </c>
-      <c r="C156" s="4" t="s">
-        <v>756</v>
       </c>
       <c r="D156" s="5">
         <v>18045.0</v>
@@ -10438,7 +10438,7 @@
       </c>
       <c r="T156" s="7"/>
       <c r="U156" s="8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="V156" s="9"/>
       <c r="W156" s="9"/>
@@ -10447,13 +10447,13 @@
     </row>
     <row r="157">
       <c r="A157" s="4" t="s">
+        <v>757</v>
+      </c>
+      <c r="B157" s="4" t="s">
         <v>758</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="C157" s="4" t="s">
         <v>759</v>
-      </c>
-      <c r="C157" s="4" t="s">
-        <v>760</v>
       </c>
       <c r="D157" s="5">
         <v>18515.0</v>
@@ -10481,11 +10481,11 @@
       </c>
       <c r="R157" s="4"/>
       <c r="S157" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T157" s="4"/>
       <c r="U157" s="8" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="V157" s="9"/>
       <c r="W157" s="9"/>
@@ -10494,10 +10494,10 @@
     </row>
     <row r="158">
       <c r="A158" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="B158" s="4" t="s">
         <v>762</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>763</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>540</v>
@@ -10526,13 +10526,13 @@
       <c r="Q158" s="4"/>
       <c r="R158" s="7"/>
       <c r="S158" s="4" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="T158" s="5">
         <v>2012.0</v>
       </c>
       <c r="U158" s="8" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="V158" s="9"/>
       <c r="W158" s="9"/>
@@ -10541,13 +10541,13 @@
     </row>
     <row r="159">
       <c r="A159" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="B159" s="4" t="s">
         <v>766</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="C159" s="4" t="s">
         <v>767</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>768</v>
       </c>
       <c r="D159" s="5">
         <v>18885.0</v>
@@ -10573,11 +10573,11 @@
       <c r="Q159" s="4"/>
       <c r="R159" s="7"/>
       <c r="S159" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T159" s="7"/>
       <c r="U159" s="8" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="V159" s="9"/>
       <c r="W159" s="9"/>
@@ -10586,10 +10586,10 @@
     </row>
     <row r="160">
       <c r="A160" s="4" t="s">
+        <v>769</v>
+      </c>
+      <c r="B160" s="4" t="s">
         <v>770</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>771</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>128</v>
@@ -10618,11 +10618,11 @@
       <c r="Q160" s="4"/>
       <c r="R160" s="7"/>
       <c r="S160" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="T160" s="4"/>
       <c r="U160" s="8" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="V160" s="9"/>
       <c r="W160" s="9"/>
@@ -10631,10 +10631,10 @@
     </row>
     <row r="161">
       <c r="A161" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="B161" s="4" t="s">
         <v>773</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>774</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>262</v>
@@ -10663,11 +10663,11 @@
       <c r="Q161" s="4"/>
       <c r="R161" s="7"/>
       <c r="S161" s="4" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="T161" s="4"/>
       <c r="U161" s="8" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="V161" s="9"/>
       <c r="W161" s="9"/>
@@ -10676,13 +10676,13 @@
     </row>
     <row r="162">
       <c r="A162" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="B162" s="4" t="s">
         <v>777</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="C162" s="4" t="s">
         <v>778</v>
-      </c>
-      <c r="C162" s="4" t="s">
-        <v>779</v>
       </c>
       <c r="D162" s="5">
         <v>18894.0</v>
@@ -10708,13 +10708,13 @@
       <c r="Q162" s="4"/>
       <c r="R162" s="7"/>
       <c r="S162" s="4" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="T162" s="5">
         <v>1972.0</v>
       </c>
       <c r="U162" s="8" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="V162" s="9"/>
       <c r="W162" s="9"/>
@@ -10723,13 +10723,13 @@
     </row>
     <row r="163">
       <c r="A163" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="B163" s="4" t="s">
         <v>782</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="C163" s="4" t="s">
         <v>783</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>784</v>
       </c>
       <c r="D163" s="5">
         <v>18796.0</v>
@@ -10755,11 +10755,11 @@
       <c r="Q163" s="4"/>
       <c r="R163" s="7"/>
       <c r="S163" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="T163" s="4"/>
       <c r="U163" s="8" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="V163" s="9"/>
       <c r="W163" s="9"/>
@@ -10768,13 +10768,13 @@
     </row>
     <row r="164">
       <c r="A164" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="B164" s="4" t="s">
         <v>786</v>
       </c>
-      <c r="B164" s="4" t="s">
-        <v>787</v>
-      </c>
       <c r="C164" s="4" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D164" s="5">
         <v>18796.0</v>
@@ -10800,11 +10800,11 @@
       <c r="Q164" s="4"/>
       <c r="R164" s="7"/>
       <c r="S164" s="4" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="T164" s="4"/>
       <c r="U164" s="8" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="V164" s="9"/>
       <c r="W164" s="9"/>
@@ -10813,13 +10813,13 @@
     </row>
     <row r="165">
       <c r="A165" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="B165" s="4" t="s">
         <v>790</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="C165" s="4" t="s">
         <v>791</v>
-      </c>
-      <c r="C165" s="4" t="s">
-        <v>792</v>
       </c>
       <c r="D165" s="5">
         <v>18897.0</v>
@@ -10845,13 +10845,13 @@
       <c r="Q165" s="4"/>
       <c r="R165" s="7"/>
       <c r="S165" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T165" s="5">
         <v>1975.0</v>
       </c>
       <c r="U165" s="8" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="V165" s="9"/>
       <c r="W165" s="9"/>
@@ -10860,13 +10860,13 @@
     </row>
     <row r="166">
       <c r="A166" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="B166" s="4" t="s">
         <v>794</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="C166" s="4" t="s">
         <v>795</v>
-      </c>
-      <c r="C166" s="4" t="s">
-        <v>796</v>
       </c>
       <c r="D166" s="5">
         <v>18907.0</v>
@@ -10894,11 +10894,11 @@
       </c>
       <c r="R166" s="4"/>
       <c r="S166" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T166" s="4"/>
       <c r="U166" s="8" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="V166" s="9"/>
       <c r="W166" s="9"/>
@@ -10907,10 +10907,10 @@
     </row>
     <row r="167">
       <c r="A167" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="B167" s="4" t="s">
         <v>798</v>
-      </c>
-      <c r="B167" s="4" t="s">
-        <v>799</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>134</v>
@@ -10939,13 +10939,13 @@
       <c r="Q167" s="4"/>
       <c r="R167" s="7"/>
       <c r="S167" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T167" s="5">
         <v>2007.0</v>
       </c>
       <c r="U167" s="8" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="V167" s="9"/>
       <c r="W167" s="9"/>
@@ -10954,13 +10954,13 @@
     </row>
     <row r="168">
       <c r="A168" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="B168" s="4" t="s">
         <v>801</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="C168" s="4" t="s">
         <v>802</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>803</v>
       </c>
       <c r="D168" s="5">
         <v>18919.0</v>
@@ -10986,13 +10986,13 @@
       <c r="Q168" s="4"/>
       <c r="R168" s="7"/>
       <c r="S168" s="4" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="T168" s="5">
         <v>2007.0</v>
       </c>
       <c r="U168" s="8" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="V168" s="9"/>
       <c r="W168" s="9"/>
@@ -11001,10 +11001,10 @@
     </row>
     <row r="169">
       <c r="A169" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="B169" s="4" t="s">
         <v>806</v>
-      </c>
-      <c r="B169" s="4" t="s">
-        <v>807</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>428</v>
@@ -11033,11 +11033,11 @@
       <c r="Q169" s="4"/>
       <c r="R169" s="7"/>
       <c r="S169" s="4" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="T169" s="4"/>
       <c r="U169" s="8" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="V169" s="9"/>
       <c r="W169" s="9"/>
@@ -11046,10 +11046,10 @@
     </row>
     <row r="170">
       <c r="A170" s="4" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>328</v>
@@ -11078,11 +11078,11 @@
       <c r="Q170" s="4"/>
       <c r="R170" s="7"/>
       <c r="S170" s="4" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="T170" s="4"/>
       <c r="U170" s="8" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="V170" s="9"/>
       <c r="W170" s="9"/>
@@ -11091,13 +11091,13 @@
     </row>
     <row r="171">
       <c r="A171" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="B171" s="4" t="s">
         <v>813</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="C171" s="4" t="s">
         <v>814</v>
-      </c>
-      <c r="C171" s="4" t="s">
-        <v>815</v>
       </c>
       <c r="D171" s="5">
         <v>18951.0</v>
@@ -11127,7 +11127,7 @@
       </c>
       <c r="T171" s="4"/>
       <c r="U171" s="8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="V171" s="9"/>
       <c r="W171" s="9"/>
@@ -11136,13 +11136,13 @@
     </row>
     <row r="172">
       <c r="A172" s="4" t="s">
+        <v>816</v>
+      </c>
+      <c r="B172" s="4" t="s">
         <v>817</v>
       </c>
-      <c r="B172" s="4" t="s">
-        <v>818</v>
-      </c>
       <c r="C172" s="4" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D172" s="5">
         <v>18951.0</v>
@@ -11168,11 +11168,11 @@
       <c r="Q172" s="4"/>
       <c r="R172" s="7"/>
       <c r="S172" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T172" s="7"/>
       <c r="U172" s="8" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="V172" s="9"/>
       <c r="W172" s="9"/>
@@ -11181,13 +11181,13 @@
     </row>
     <row r="173">
       <c r="A173" s="4" t="s">
+        <v>819</v>
+      </c>
+      <c r="B173" s="4" t="s">
         <v>820</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="C173" s="4" t="s">
         <v>821</v>
-      </c>
-      <c r="C173" s="4" t="s">
-        <v>822</v>
       </c>
       <c r="D173" s="5">
         <v>18815.0</v>
@@ -11213,13 +11213,13 @@
       <c r="Q173" s="4"/>
       <c r="R173" s="4"/>
       <c r="S173" s="4" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="T173" s="5">
         <v>2007.0</v>
       </c>
       <c r="U173" s="8" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="V173" s="9"/>
       <c r="W173" s="9"/>
@@ -11228,10 +11228,10 @@
     </row>
     <row r="174">
       <c r="A174" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="B174" s="4" t="s">
         <v>825</v>
-      </c>
-      <c r="B174" s="4" t="s">
-        <v>826</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>149</v>
@@ -11260,11 +11260,11 @@
       <c r="Q174" s="4"/>
       <c r="R174" s="7"/>
       <c r="S174" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="T174" s="4"/>
       <c r="U174" s="8" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="V174" s="9"/>
       <c r="W174" s="9"/>
@@ -11273,13 +11273,13 @@
     </row>
     <row r="175">
       <c r="A175" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="B175" s="4" t="s">
         <v>828</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="C175" s="4" t="s">
         <v>829</v>
-      </c>
-      <c r="C175" s="4" t="s">
-        <v>830</v>
       </c>
       <c r="D175" s="5">
         <v>18960.0</v>
@@ -11305,11 +11305,11 @@
       <c r="Q175" s="4"/>
       <c r="R175" s="7"/>
       <c r="S175" s="4" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="T175" s="4"/>
       <c r="U175" s="8" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="V175" s="9"/>
       <c r="W175" s="9"/>
@@ -11318,13 +11318,13 @@
     </row>
     <row r="176">
       <c r="A176" s="4" t="s">
+        <v>832</v>
+      </c>
+      <c r="B176" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="C176" s="4" t="s">
         <v>834</v>
-      </c>
-      <c r="C176" s="4" t="s">
-        <v>835</v>
       </c>
       <c r="D176" s="5">
         <v>18971.0</v>
@@ -11350,11 +11350,11 @@
       <c r="Q176" s="4"/>
       <c r="R176" s="7"/>
       <c r="S176" s="4" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="T176" s="4"/>
       <c r="U176" s="8" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="V176" s="9"/>
       <c r="W176" s="9"/>
@@ -11363,13 +11363,13 @@
     </row>
     <row r="177">
       <c r="A177" s="4" t="s">
+        <v>837</v>
+      </c>
+      <c r="B177" s="4" t="s">
         <v>838</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="C177" s="4" t="s">
         <v>839</v>
-      </c>
-      <c r="C177" s="4" t="s">
-        <v>840</v>
       </c>
       <c r="D177" s="5">
         <v>18972.0</v>
@@ -11395,11 +11395,11 @@
       <c r="Q177" s="4"/>
       <c r="R177" s="7"/>
       <c r="S177" s="4" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="T177" s="4"/>
       <c r="U177" s="8" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="V177" s="9"/>
       <c r="W177" s="9"/>
@@ -11408,10 +11408,10 @@
     </row>
     <row r="178">
       <c r="A178" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="B178" s="4" t="s">
         <v>843</v>
-      </c>
-      <c r="B178" s="4" t="s">
-        <v>844</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>242</v>
@@ -11440,13 +11440,13 @@
       <c r="Q178" s="4"/>
       <c r="R178" s="7"/>
       <c r="S178" s="4" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="T178" s="5">
         <v>2008.0</v>
       </c>
       <c r="U178" s="8" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="V178" s="9"/>
       <c r="W178" s="9"/>
@@ -11455,10 +11455,10 @@
     </row>
     <row r="179">
       <c r="A179" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="B179" s="4" t="s">
         <v>847</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>848</v>
       </c>
       <c r="C179" s="4" t="s">
         <v>242</v>
@@ -11487,11 +11487,11 @@
       <c r="Q179" s="4"/>
       <c r="R179" s="7"/>
       <c r="S179" s="4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T179" s="7"/>
       <c r="U179" s="8" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="V179" s="9"/>
       <c r="W179" s="9"/>
@@ -11500,13 +11500,13 @@
     </row>
     <row r="180">
       <c r="A180" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="B180" s="4" t="s">
         <v>850</v>
       </c>
-      <c r="B180" s="4" t="s">
+      <c r="C180" s="4" t="s">
         <v>851</v>
-      </c>
-      <c r="C180" s="4" t="s">
-        <v>852</v>
       </c>
       <c r="D180" s="5">
         <v>18834.0</v>
@@ -11538,7 +11538,7 @@
         <v>1951.0</v>
       </c>
       <c r="U180" s="8" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="V180" s="9"/>
       <c r="W180" s="9"/>
@@ -11547,13 +11547,13 @@
     </row>
     <row r="181">
       <c r="A181" s="4" t="s">
+        <v>853</v>
+      </c>
+      <c r="B181" s="4" t="s">
         <v>854</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="C181" s="4" t="s">
         <v>855</v>
-      </c>
-      <c r="C181" s="4" t="s">
-        <v>856</v>
       </c>
       <c r="D181" s="5">
         <v>19011.0</v>
@@ -11579,11 +11579,11 @@
       <c r="Q181" s="4"/>
       <c r="R181" s="7"/>
       <c r="S181" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="T181" s="4"/>
       <c r="U181" s="8" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="V181" s="9"/>
       <c r="W181" s="9"/>
@@ -11592,13 +11592,13 @@
     </row>
     <row r="182">
       <c r="A182" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="B182" s="4" t="s">
         <v>859</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="C182" s="4" t="s">
         <v>860</v>
-      </c>
-      <c r="C182" s="4" t="s">
-        <v>861</v>
       </c>
       <c r="D182" s="5">
         <v>19012.0</v>
@@ -11626,11 +11626,11 @@
       </c>
       <c r="R182" s="4"/>
       <c r="S182" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="T182" s="4"/>
       <c r="U182" s="8" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="V182" s="9"/>
       <c r="W182" s="9"/>
@@ -11639,13 +11639,13 @@
     </row>
     <row r="183">
       <c r="A183" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="B183" s="4" t="s">
         <v>863</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="C183" s="4" t="s">
         <v>864</v>
-      </c>
-      <c r="C183" s="4" t="s">
-        <v>865</v>
       </c>
       <c r="D183" s="5">
         <v>19072.0</v>
@@ -11671,11 +11671,11 @@
       <c r="Q183" s="4"/>
       <c r="R183" s="7"/>
       <c r="S183" s="4" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="T183" s="4"/>
       <c r="U183" s="8" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="V183" s="9"/>
       <c r="W183" s="9"/>
@@ -11684,13 +11684,13 @@
     </row>
     <row r="184">
       <c r="A184" s="4" t="s">
+        <v>867</v>
+      </c>
+      <c r="B184" s="4" t="s">
         <v>868</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="C184" s="4" t="s">
         <v>869</v>
-      </c>
-      <c r="C184" s="4" t="s">
-        <v>870</v>
       </c>
       <c r="D184" s="5">
         <v>19173.0</v>
@@ -11716,13 +11716,13 @@
       <c r="Q184" s="4"/>
       <c r="R184" s="7"/>
       <c r="S184" s="4" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="T184" s="5">
         <v>2007.0</v>
       </c>
       <c r="U184" s="8" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="V184" s="9"/>
       <c r="W184" s="9"/>
@@ -11731,13 +11731,13 @@
     </row>
     <row r="185">
       <c r="A185" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="B185" s="4" t="s">
         <v>873</v>
       </c>
-      <c r="B185" s="4" t="s">
-        <v>874</v>
-      </c>
       <c r="C185" s="4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D185" s="5">
         <v>19173.0</v>
@@ -11767,7 +11767,7 @@
       </c>
       <c r="T185" s="7"/>
       <c r="U185" s="8" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="V185" s="9"/>
       <c r="W185" s="9"/>
@@ -11776,13 +11776,13 @@
     </row>
     <row r="186">
       <c r="A186" s="4" t="s">
+        <v>875</v>
+      </c>
+      <c r="B186" s="4" t="s">
         <v>876</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="C186" s="4" t="s">
         <v>877</v>
-      </c>
-      <c r="C186" s="4" t="s">
-        <v>878</v>
       </c>
       <c r="D186" s="5">
         <v>19246.0</v>
@@ -11808,11 +11808,11 @@
       <c r="Q186" s="4"/>
       <c r="R186" s="7"/>
       <c r="S186" s="4" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="T186" s="4"/>
       <c r="U186" s="8" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="V186" s="9"/>
       <c r="W186" s="9"/>
@@ -11821,13 +11821,13 @@
     </row>
     <row r="187">
       <c r="A187" s="4" t="s">
+        <v>880</v>
+      </c>
+      <c r="B187" s="4" t="s">
         <v>881</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="C187" s="4" t="s">
         <v>882</v>
-      </c>
-      <c r="C187" s="4" t="s">
-        <v>883</v>
       </c>
       <c r="D187" s="5">
         <v>16046.0</v>
@@ -11857,7 +11857,7 @@
       </c>
       <c r="T187" s="7"/>
       <c r="U187" s="8" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="V187" s="9"/>
       <c r="W187" s="9"/>
@@ -11866,10 +11866,10 @@
     </row>
     <row r="188">
       <c r="A188" s="4" t="s">
+        <v>884</v>
+      </c>
+      <c r="B188" s="4" t="s">
         <v>885</v>
-      </c>
-      <c r="B188" s="4" t="s">
-        <v>886</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>184</v>
@@ -11898,13 +11898,13 @@
       <c r="Q188" s="4"/>
       <c r="R188" s="4"/>
       <c r="S188" s="4" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="T188" s="5">
         <v>2005.0</v>
       </c>
       <c r="U188" s="8" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="V188" s="9"/>
       <c r="W188" s="9"/>
@@ -11913,13 +11913,13 @@
     </row>
     <row r="189">
       <c r="A189" s="4" t="s">
+        <v>888</v>
+      </c>
+      <c r="B189" s="4" t="s">
         <v>889</v>
       </c>
-      <c r="B189" s="4" t="s">
-        <v>890</v>
-      </c>
       <c r="C189" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D189" s="5">
         <v>16365.0</v>
@@ -11945,13 +11945,13 @@
       <c r="Q189" s="4"/>
       <c r="R189" s="4"/>
       <c r="S189" s="4" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="T189" s="5">
         <v>1972.0</v>
       </c>
       <c r="U189" s="8" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="V189" s="9"/>
       <c r="W189" s="9"/>
@@ -11960,13 +11960,13 @@
     </row>
     <row r="190">
       <c r="A190" s="4" t="s">
+        <v>892</v>
+      </c>
+      <c r="B190" s="4" t="s">
         <v>893</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="C190" s="4" t="s">
         <v>894</v>
-      </c>
-      <c r="C190" s="4" t="s">
-        <v>895</v>
       </c>
       <c r="D190" s="5">
         <v>17637.0</v>
@@ -11994,13 +11994,13 @@
       </c>
       <c r="R190" s="4"/>
       <c r="S190" s="4" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="T190" s="5">
         <v>1999.0</v>
       </c>
       <c r="U190" s="8" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="V190" s="9"/>
       <c r="W190" s="9"/>
@@ -12009,13 +12009,13 @@
     </row>
     <row r="191">
       <c r="A191" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="B191" s="4" t="s">
         <v>898</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="C191" s="4" t="s">
         <v>899</v>
-      </c>
-      <c r="C191" s="4" t="s">
-        <v>900</v>
       </c>
       <c r="D191" s="5">
         <v>16042.0</v>
@@ -12045,11 +12045,11 @@
         <v>88</v>
       </c>
       <c r="S191" s="4" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="T191" s="4"/>
       <c r="U191" s="8" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="V191" s="9"/>
       <c r="W191" s="9"/>
@@ -12058,10 +12058,10 @@
     </row>
     <row r="192">
       <c r="A192" s="4" t="s">
+        <v>902</v>
+      </c>
+      <c r="B192" s="4" t="s">
         <v>903</v>
-      </c>
-      <c r="B192" s="4" t="s">
-        <v>904</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>128</v>
@@ -12092,11 +12092,11 @@
       </c>
       <c r="R192" s="4"/>
       <c r="S192" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="T192" s="4"/>
       <c r="U192" s="8" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="V192" s="9"/>
       <c r="W192" s="9"/>
@@ -12105,10 +12105,10 @@
     </row>
     <row r="193">
       <c r="A193" s="4" t="s">
+        <v>906</v>
+      </c>
+      <c r="B193" s="4" t="s">
         <v>907</v>
-      </c>
-      <c r="B193" s="4" t="s">
-        <v>908</v>
       </c>
       <c r="C193" s="4" t="s">
         <v>553</v>
@@ -12139,11 +12139,11 @@
       </c>
       <c r="R193" s="4"/>
       <c r="S193" s="4" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="T193" s="4"/>
       <c r="U193" s="8" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="V193" s="9"/>
       <c r="W193" s="9"/>
@@ -12152,13 +12152,13 @@
     </row>
     <row r="194">
       <c r="A194" s="4" t="s">
+        <v>910</v>
+      </c>
+      <c r="B194" s="4" t="s">
         <v>911</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="C194" s="4" t="s">
         <v>912</v>
-      </c>
-      <c r="C194" s="4" t="s">
-        <v>913</v>
       </c>
       <c r="D194" s="5">
         <v>19554.0</v>
@@ -12186,11 +12186,11 @@
       </c>
       <c r="R194" s="4"/>
       <c r="S194" s="4" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="T194" s="4"/>
       <c r="U194" s="8" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="V194" s="9"/>
       <c r="W194" s="9"/>
@@ -12199,13 +12199,13 @@
     </row>
     <row r="195">
       <c r="A195" s="4" t="s">
+        <v>915</v>
+      </c>
+      <c r="B195" s="4" t="s">
         <v>916</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="C195" s="4" t="s">
         <v>917</v>
-      </c>
-      <c r="C195" s="4" t="s">
-        <v>918</v>
       </c>
       <c r="D195" s="5">
         <v>18926.0</v>
@@ -12235,11 +12235,11 @@
         <v>88</v>
       </c>
       <c r="S195" s="4" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="T195" s="4"/>
       <c r="U195" s="8" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="V195" s="9"/>
       <c r="W195" s="9"/>
@@ -12248,10 +12248,10 @@
     </row>
     <row r="196">
       <c r="A196" s="4" t="s">
+        <v>920</v>
+      </c>
+      <c r="B196" s="4" t="s">
         <v>921</v>
-      </c>
-      <c r="B196" s="4" t="s">
-        <v>922</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>428</v>
@@ -12271,7 +12271,7 @@
         <v>24</v>
       </c>
       <c r="N196" s="4" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="O196" s="4"/>
       <c r="P196" s="4" t="s">
@@ -12280,11 +12280,11 @@
       <c r="Q196" s="4"/>
       <c r="R196" s="4"/>
       <c r="S196" s="4" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="T196" s="4"/>
       <c r="U196" s="8" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="V196" s="9"/>
       <c r="W196" s="9"/>
@@ -12293,13 +12293,13 @@
     </row>
     <row r="197">
       <c r="A197" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="B197" s="4" t="s">
         <v>926</v>
       </c>
-      <c r="B197" s="4" t="s">
-        <v>927</v>
-      </c>
       <c r="C197" s="4" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D197" s="5">
         <v>18971.0</v>
@@ -12325,11 +12325,11 @@
       <c r="Q197" s="4"/>
       <c r="R197" s="4"/>
       <c r="S197" s="4" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="T197" s="4"/>
       <c r="U197" s="8" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="V197" s="9"/>
       <c r="W197" s="9"/>
@@ -12338,10 +12338,10 @@
     </row>
     <row r="198">
       <c r="A198" s="4" t="s">
+        <v>929</v>
+      </c>
+      <c r="B198" s="4" t="s">
         <v>930</v>
-      </c>
-      <c r="B198" s="4" t="s">
-        <v>931</v>
       </c>
       <c r="C198" s="4" t="s">
         <v>242</v>
@@ -12372,13 +12372,13 @@
       </c>
       <c r="R198" s="4"/>
       <c r="S198" s="4" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="T198" s="5">
         <v>1957.0</v>
       </c>
       <c r="U198" s="8" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="V198" s="9"/>
       <c r="W198" s="9"/>
@@ -12390,10 +12390,10 @@
         <v>137</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D199" s="5">
         <v>19012.0</v>
@@ -12419,13 +12419,13 @@
       <c r="Q199" s="4"/>
       <c r="R199" s="4"/>
       <c r="S199" s="4" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="T199" s="5">
         <v>1998.0</v>
       </c>
       <c r="U199" s="8" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="V199" s="9"/>
       <c r="W199" s="9"/>
@@ -12434,13 +12434,13 @@
     </row>
     <row r="200">
       <c r="A200" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="B200" s="4" t="s">
         <v>937</v>
       </c>
-      <c r="B200" s="4" t="s">
+      <c r="C200" s="4" t="s">
         <v>938</v>
-      </c>
-      <c r="C200" s="4" t="s">
-        <v>939</v>
       </c>
       <c r="D200" s="5">
         <v>19079.0</v>
@@ -12466,11 +12466,11 @@
       <c r="Q200" s="4"/>
       <c r="R200" s="4"/>
       <c r="S200" s="4" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="T200" s="4"/>
       <c r="U200" s="8" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="V200" s="9"/>
       <c r="W200" s="9"/>
@@ -12479,10 +12479,10 @@
     </row>
     <row r="201">
       <c r="A201" s="4" t="s">
+        <v>941</v>
+      </c>
+      <c r="B201" s="4" t="s">
         <v>942</v>
-      </c>
-      <c r="B201" s="4" t="s">
-        <v>943</v>
       </c>
       <c r="C201" s="4" t="s">
         <v>482</v>
@@ -12515,7 +12515,7 @@
       </c>
       <c r="T201" s="7"/>
       <c r="U201" s="8" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="V201" s="9"/>
       <c r="W201" s="9"/>
@@ -12524,10 +12524,10 @@
     </row>
     <row r="202">
       <c r="A202" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="B202" s="4" t="s">
         <v>945</v>
-      </c>
-      <c r="B202" s="4" t="s">
-        <v>946</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>230</v>
@@ -12562,7 +12562,7 @@
         <v>2004.0</v>
       </c>
       <c r="U202" s="8" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="V202" s="9"/>
       <c r="W202" s="9"/>
@@ -12571,10 +12571,10 @@
     </row>
     <row r="203">
       <c r="A203" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="B203" s="4" t="s">
         <v>948</v>
-      </c>
-      <c r="B203" s="4" t="s">
-        <v>949</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>230</v>
@@ -12603,11 +12603,11 @@
       <c r="Q203" s="4"/>
       <c r="R203" s="4"/>
       <c r="S203" s="4" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="T203" s="4"/>
       <c r="U203" s="8" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="V203" s="9"/>
       <c r="W203" s="9"/>
@@ -12616,13 +12616,13 @@
     </row>
     <row r="204">
       <c r="A204" s="4" t="s">
+        <v>951</v>
+      </c>
+      <c r="B204" s="4" t="s">
         <v>952</v>
       </c>
-      <c r="B204" s="4" t="s">
-        <v>953</v>
-      </c>
       <c r="C204" s="4" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D204" s="5">
         <v>18960.0</v>
@@ -12648,11 +12648,11 @@
       <c r="Q204" s="6"/>
       <c r="R204" s="7"/>
       <c r="S204" s="4" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="T204" s="4"/>
       <c r="U204" s="8" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="V204" s="9"/>
       <c r="W204" s="9"/>
@@ -12661,13 +12661,13 @@
     </row>
     <row r="205">
       <c r="A205" s="4" t="s">
+        <v>955</v>
+      </c>
+      <c r="B205" s="4" t="s">
         <v>956</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="C205" s="4" t="s">
         <v>957</v>
-      </c>
-      <c r="C205" s="4" t="s">
-        <v>958</v>
       </c>
       <c r="D205" s="5">
         <v>17161.0</v>
@@ -12693,11 +12693,11 @@
       <c r="Q205" s="4"/>
       <c r="R205" s="7"/>
       <c r="S205" s="4" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="T205" s="4"/>
       <c r="U205" s="8" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="V205" s="9"/>
       <c r="W205" s="9"/>

</xml_diff>